<commit_message>
delivery address codea added
</commit_message>
<xml_diff>
--- a/jenkinTest/Data/GoogleSearch.xlsx
+++ b/jenkinTest/Data/GoogleSearch.xlsx
@@ -3,23 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valmiki\git\UAT\jenkinTest\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17835" windowHeight="2715" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:R7"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Username</t>
   </si>
@@ -31,6 +28,48 @@
   </si>
   <si>
     <t>Test@123</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Address 1</t>
+  </si>
+  <si>
+    <t>Address 2</t>
+  </si>
+  <si>
+    <t>Landmark</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Pin Code</t>
+  </si>
+  <si>
+    <t>Mobile Number</t>
+  </si>
+  <si>
+    <t>Valmiki</t>
+  </si>
+  <si>
+    <t>203, Akshar Bluechip IT Park,</t>
+  </si>
+  <si>
+    <t>Turbhe MIDC</t>
+  </si>
+  <si>
+    <t>Turbhe</t>
+  </si>
+  <si>
+    <t>New Mumbai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maharashtra </t>
   </si>
 </sst>
 </file>
@@ -75,12 +114,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -90,10 +144,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -372,7 +428,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -404,4 +462,82 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="4">
+        <v>400705</v>
+      </c>
+      <c r="H2" s="4">
+        <v>2262596124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>